<commit_message>
fix: adicionado o valor de 25000 em decoração
</commit_message>
<xml_diff>
--- a/Planilha casamento Guga e Camilla.xlsx
+++ b/Planilha casamento Guga e Camilla.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6574CC44-C12B-45EE-A32B-4C9D98500C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{6574CC44-C12B-45EE-A32B-4C9D98500C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{172A64F8-FF89-44B7-9F83-B0DA77A00EB1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orçamento de casamento" sheetId="1" r:id="rId1"/>
@@ -1205,6 +1205,9 @@
     <xf numFmtId="4" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="167" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
@@ -1219,9 +1222,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -1376,11 +1376,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1392,7 +1388,13 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1412,688 +1414,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2120,49 +1440,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -2176,149 +1453,10 @@
         <color theme="3" tint="-0.749992370372631"/>
         <name val="Arial"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
       </font>
       <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2344,7 +1482,11 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -2355,36 +1497,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.749992370372631"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2474,7 +1588,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2490,12 +1604,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2526,6 +1634,26 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2549,6 +1677,72 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2643,7 +1837,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2659,12 +1853,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2695,6 +1883,26 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2718,6 +1926,72 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2812,7 +2086,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2828,12 +2102,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2864,6 +2132,26 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2887,6 +2175,72 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3133,7 +2487,11 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -3145,13 +2503,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3177,6 +2529,26 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -3196,6 +2568,68 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3285,7 +2719,11 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -3297,13 +2735,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3329,6 +2761,26 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -3348,6 +2800,68 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3437,7 +2951,11 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -3449,13 +2967,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3481,6 +2993,26 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -3500,6 +3032,68 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3589,7 +3183,11 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -3601,13 +3199,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3633,6 +3225,26 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -3652,6 +3264,68 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3742,6 +3416,173 @@
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -3803,6 +3644,165 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="3" tint="-0.749992370372631"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4432,7 +4432,7 @@
                   <c:v>1575</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>720</c:v>
+                  <c:v>20720</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>850</c:v>
@@ -9895,8 +9895,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="189238" y="1749996"/>
-          <a:ext cx="8751189" cy="0"/>
+          <a:off x="189238" y="1759521"/>
+          <a:ext cx="8756904" cy="0"/>
           <a:chOff x="189238" y="1672450"/>
           <a:chExt cx="6661192" cy="0"/>
         </a:xfrm>
@@ -10003,8 +10003,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="189238" y="7185596"/>
-          <a:ext cx="8751189" cy="0"/>
+          <a:off x="189238" y="7143686"/>
+          <a:ext cx="8756904" cy="0"/>
           <a:chOff x="189238" y="1672450"/>
           <a:chExt cx="6661192" cy="0"/>
         </a:xfrm>
@@ -10111,8 +10111,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="189238" y="11272520"/>
-          <a:ext cx="8751189" cy="0"/>
+          <a:off x="189238" y="11184890"/>
+          <a:ext cx="8756904" cy="0"/>
           <a:chOff x="189238" y="1672450"/>
           <a:chExt cx="6661192" cy="0"/>
         </a:xfrm>
@@ -10219,8 +10219,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="189238" y="13093700"/>
-          <a:ext cx="8751189" cy="0"/>
+          <a:off x="189238" y="12994640"/>
+          <a:ext cx="8756904" cy="0"/>
           <a:chOff x="189238" y="1672450"/>
           <a:chExt cx="6661192" cy="0"/>
         </a:xfrm>
@@ -10327,8 +10327,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="190921" y="17208500"/>
-          <a:ext cx="8808299" cy="0"/>
+          <a:off x="190921" y="17071340"/>
+          <a:ext cx="8819729" cy="0"/>
           <a:chOff x="189238" y="1672450"/>
           <a:chExt cx="6661192" cy="0"/>
         </a:xfrm>
@@ -10435,8 +10435,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="190921" y="19685000"/>
-          <a:ext cx="8808299" cy="0"/>
+          <a:off x="190921" y="19528790"/>
+          <a:ext cx="8819729" cy="0"/>
           <a:chOff x="189238" y="1672450"/>
           <a:chExt cx="6661192" cy="0"/>
         </a:xfrm>
@@ -10543,8 +10543,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="190921" y="22755860"/>
-          <a:ext cx="8808299" cy="0"/>
+          <a:off x="190921" y="22576790"/>
+          <a:ext cx="8819729" cy="0"/>
           <a:chOff x="189238" y="1672450"/>
           <a:chExt cx="6661192" cy="0"/>
         </a:xfrm>
@@ -10651,8 +10651,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="190921" y="25471120"/>
-          <a:ext cx="8808299" cy="0"/>
+          <a:off x="190921" y="25267285"/>
+          <a:ext cx="8819729" cy="0"/>
           <a:chOff x="189238" y="1672450"/>
           <a:chExt cx="6661192" cy="0"/>
         </a:xfrm>
@@ -10759,8 +10759,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="190921" y="28295600"/>
-          <a:ext cx="8808299" cy="0"/>
+          <a:off x="190921" y="28063190"/>
+          <a:ext cx="8819729" cy="0"/>
           <a:chOff x="189238" y="1672450"/>
           <a:chExt cx="6661192" cy="0"/>
         </a:xfrm>
@@ -10867,8 +10867,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="190921" y="30444440"/>
-          <a:ext cx="8808299" cy="0"/>
+          <a:off x="190921" y="30196790"/>
+          <a:ext cx="8819729" cy="0"/>
           <a:chOff x="189238" y="1672450"/>
           <a:chExt cx="6661192" cy="0"/>
         </a:xfrm>
@@ -10958,10 +10958,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CATEGORIA" totalsRowLabel="Despesas totais" dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="45" totalsRowDxfId="44">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CATEGORIA" totalsRowLabel="Despesas totais" dataDxfId="117" totalsRowDxfId="116"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="115" totalsRowDxfId="114"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="113" totalsRowDxfId="112"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="111" totalsRowDxfId="110">
       <calculatedColumnFormula>ResumoDoOrçamento[[#This Row],[ESTIMADO]]-ResumoDoOrçamento[[#This Row],[REAL]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10975,7 +10975,7 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Viagem" displayName="Viagem" ref="B81:E85" totalsRowCount="1" headerRowDxfId="65" dataDxfId="64" totalsRowDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Viagem" displayName="Viagem" ref="B81:E85" totalsRowCount="1" headerRowDxfId="25" dataDxfId="24" totalsRowDxfId="23">
   <autoFilter ref="B81:E84" xr:uid="{00000000-0009-0000-0100-000014000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -10983,10 +10983,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="CATEGORIA" totalsRowLabel="Total de viagens/transporte" dataDxfId="62" totalsRowDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="61" totalsRowDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="59" totalsRowDxfId="32">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="CATEGORIA" totalsRowLabel="Total de viagens/transporte" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15">
       <calculatedColumnFormula>Despesas!$C82-Despesas!$D82</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -11000,7 +11000,7 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="OutrasDespesas" displayName="OutrasDespesas" ref="B87:E98" totalsRowCount="1" headerRowDxfId="58" dataDxfId="57" totalsRowDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="OutrasDespesas" displayName="OutrasDespesas" ref="B87:E98" totalsRowCount="1" headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="12">
   <autoFilter ref="B87:E97" xr:uid="{00000000-0009-0000-0100-000015000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -11008,10 +11008,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="CATEGORIA" totalsRowLabel="Total de outras despesas" dataDxfId="55" totalsRowDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="53" totalsRowDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="36">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="CATEGORIA" totalsRowLabel="Total de outras despesas" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4">
       <calculatedColumnFormula>Despesas!$C88-Despesas!$D88</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -11025,7 +11025,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Vestuário" displayName="Vestuário" ref="B4:E18" totalsRowCount="1" headerRowDxfId="117" dataDxfId="116" totalsRowDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Vestuário" displayName="Vestuário" ref="B4:E18" totalsRowCount="1" headerRowDxfId="109" dataDxfId="108" totalsRowDxfId="107">
   <autoFilter ref="B4:E17" xr:uid="{00000000-0009-0000-0100-00000C000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -11033,10 +11033,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CATEGORIA" totalsRowLabel="Total das roupas" dataDxfId="43" totalsRowDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CATEGORIA" totalsRowLabel="Total das roupas" dataDxfId="106" totalsRowDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="104" totalsRowDxfId="103"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="102" totalsRowDxfId="101"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="100" totalsRowDxfId="99">
       <calculatedColumnFormula>Despesas!$C5-Despesas!$D5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -11050,7 +11050,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Recepção" displayName="Recepção" ref="B20:E29" totalsRowCount="1" headerRowDxfId="114" dataDxfId="113" totalsRowDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Recepção" displayName="Recepção" ref="B20:E29" totalsRowCount="1" headerRowDxfId="98" dataDxfId="97" totalsRowDxfId="96">
   <autoFilter ref="B20:E28" xr:uid="{00000000-0009-0000-0100-00000D000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -11058,10 +11058,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="CATEGORIA" totalsRowLabel="Total da festa" dataDxfId="111" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="110" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="109" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="108" totalsRowDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="CATEGORIA" totalsRowLabel="Total da festa" dataDxfId="95" totalsRowDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="93" totalsRowDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="91" totalsRowDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="89" totalsRowDxfId="88">
       <calculatedColumnFormula>Despesas!$C21-Despesas!$D21</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -11075,7 +11075,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Música" displayName="Música" ref="B32:E35" totalsRowCount="1" headerRowDxfId="107" dataDxfId="106" totalsRowDxfId="105">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Música" displayName="Música" ref="B32:E35" totalsRowCount="1" headerRowDxfId="87" dataDxfId="86" totalsRowDxfId="85">
   <autoFilter ref="B32:E34" xr:uid="{00000000-0009-0000-0100-00000E000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -11083,10 +11083,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="CATEGORIA" totalsRowLabel="Total de música/entretenimento" dataDxfId="104" totalsRowDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="103" totalsRowDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="102" totalsRowDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="101" totalsRowDxfId="12">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="CATEGORIA" totalsRowLabel="Total de música/entretenimento" dataDxfId="84" totalsRowDxfId="83"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="82" totalsRowDxfId="81"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="80" totalsRowDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="78" totalsRowDxfId="77">
       <calculatedColumnFormula>Despesas!$C33-Despesas!$D33</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -11100,7 +11100,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Impressão" displayName="Impressão" ref="B37:E47" totalsRowCount="1" headerRowDxfId="100" dataDxfId="99" totalsRowDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Impressão" displayName="Impressão" ref="B37:E47" totalsRowCount="1" headerRowDxfId="76" dataDxfId="75" totalsRowDxfId="74">
   <autoFilter ref="B37:E46" xr:uid="{00000000-0009-0000-0100-00000F000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -11108,10 +11108,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="CATEGORIA" totalsRowLabel="Total de impressões/papelaria" dataDxfId="97" totalsRowDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="96" totalsRowDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="95" totalsRowDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="94" totalsRowDxfId="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="CATEGORIA" totalsRowLabel="Total de impressões/papelaria" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="67" totalsRowDxfId="66">
       <calculatedColumnFormula>Despesas!$C38-Despesas!$D38</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -11125,7 +11125,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Fotografia" displayName="Fotografia" ref="B49:E54" totalsRowCount="1" headerRowDxfId="93" dataDxfId="92" totalsRowDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Fotografia" displayName="Fotografia" ref="B49:E54" totalsRowCount="1" headerRowDxfId="65" dataDxfId="64" totalsRowDxfId="63">
   <autoFilter ref="B49:E53" xr:uid="{00000000-0009-0000-0100-000010000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -11133,10 +11133,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="CATEGORIA" totalsRowLabel="Total de fotografia" dataDxfId="90" totalsRowDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="89" totalsRowDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="88" totalsRowDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="87" totalsRowDxfId="20">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="CATEGORIA" totalsRowLabel="Total de fotografia" dataDxfId="62" totalsRowDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="56" totalsRowDxfId="55">
       <calculatedColumnFormula>Despesas!$C50-Despesas!$D50</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -11150,7 +11150,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Decorações" displayName="Decorações" ref="B56:E62" totalsRowCount="1" headerRowDxfId="86" dataDxfId="85" totalsRowDxfId="84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Decorações" displayName="Decorações" ref="B56:E62" totalsRowCount="1" headerRowDxfId="54" dataDxfId="53" totalsRowDxfId="52">
   <autoFilter ref="B56:E61" xr:uid="{00000000-0009-0000-0100-000011000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -11158,10 +11158,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="CATEGORIA" totalsRowLabel="Total de decoração" dataDxfId="83" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="82" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="81" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="80" totalsRowDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="CATEGORIA" totalsRowLabel="Total de decoração" dataDxfId="51" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="48" totalsRowDxfId="0">
       <calculatedColumnFormula>Despesas!$C57-Despesas!$D57</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -11175,7 +11175,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Flores" displayName="Flores" ref="B65:E71" totalsRowCount="1" headerRowDxfId="79" dataDxfId="78" totalsRowDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Flores" displayName="Flores" ref="B65:E71" totalsRowCount="1" headerRowDxfId="47" dataDxfId="46" totalsRowDxfId="45">
   <autoFilter ref="B65:E70" xr:uid="{00000000-0009-0000-0100-000012000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -11183,10 +11183,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="CATEGORIA" totalsRowLabel="Total de flores" dataDxfId="76" totalsRowDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="75" totalsRowDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="74" totalsRowDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="73" totalsRowDxfId="24">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="CATEGORIA" totalsRowLabel="Total de flores" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37">
       <calculatedColumnFormula>Despesas!$C66-Despesas!$D66</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -11200,7 +11200,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Presentes" displayName="Presentes" ref="B73:E79" totalsRowCount="1" headerRowDxfId="72" dataDxfId="71" totalsRowDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Presentes" displayName="Presentes" ref="B73:E79" totalsRowCount="1" headerRowDxfId="36" dataDxfId="35" totalsRowDxfId="34">
   <autoFilter ref="B73:E78" xr:uid="{00000000-0009-0000-0100-000013000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -11208,10 +11208,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="CATEGORIA" totalsRowLabel="Total de presentes" dataDxfId="69" totalsRowDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="68" totalsRowDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="67" totalsRowDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="66" totalsRowDxfId="28">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="CATEGORIA" totalsRowLabel="Total de presentes" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="ACIMA/ABAIXO/RESTANTE" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26">
       <calculatedColumnFormula>Despesas!$C74-Despesas!$D74</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -11473,14 +11473,14 @@
     <row r="4" spans="1:5" ht="28.2" customHeight="1">
       <c r="B4" s="40">
         <f ca="1">TODAY()+365</f>
-        <v>46409</v>
+        <v>46414</v>
       </c>
       <c r="C4" s="40"/>
-      <c r="D4" s="48">
+      <c r="D4" s="43">
         <f ca="1">B4-TODAY()</f>
         <v>365</v>
       </c>
-      <c r="E4" s="43"/>
+      <c r="E4" s="44"/>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="25.95" customHeight="1">
       <c r="A5" s="4"/>
@@ -11589,15 +11589,15 @@
       </c>
       <c r="C11" s="27">
         <f>Total_de_Decoração_est</f>
-        <v>20000</v>
+        <v>25000</v>
       </c>
       <c r="D11" s="27">
         <f>Total_de_Decoração_real</f>
-        <v>720</v>
+        <v>20720</v>
       </c>
       <c r="E11" s="27">
         <f>ResumoDoOrçamento[[#This Row],[ESTIMADO]]-ResumoDoOrçamento[[#This Row],[REAL]]</f>
-        <v>19280</v>
+        <v>4280</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="25.95" customHeight="1">
@@ -11674,15 +11674,15 @@
       </c>
       <c r="C16" s="37">
         <f>SUBTOTAL(109,ResumoDoOrçamento[ESTIMADO])</f>
-        <v>54875</v>
+        <v>59875</v>
       </c>
       <c r="D16" s="37">
         <f>SUBTOTAL(109,ResumoDoOrçamento[REAL])</f>
-        <v>5915</v>
+        <v>25915</v>
       </c>
       <c r="E16" s="37">
         <f>SUBTOTAL(109,ResumoDoOrçamento[ACIMA/ABAIXO])</f>
-        <v>48960</v>
+        <v>33960</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="25.95" customHeight="1">
@@ -11840,7 +11840,7 @@
   <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.25" customHeight="1"/>
@@ -11854,27 +11854,27 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" customHeight="1">
       <c r="A1" s="8"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:6" ht="100.2" customHeight="1">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" spans="1:6" ht="40.200000000000003" customHeight="1">
       <c r="A3" s="8"/>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
     </row>
     <row r="4" spans="1:6" ht="25.95" customHeight="1">
       <c r="A4" s="10"/>
@@ -12110,12 +12110,12 @@
     </row>
     <row r="19" spans="1:5" ht="40.200000000000003" customHeight="1">
       <c r="A19" s="8"/>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
     </row>
     <row r="20" spans="1:5" ht="25.95" customHeight="1">
       <c r="A20" s="4"/>
@@ -12280,12 +12280,12 @@
     </row>
     <row r="31" spans="1:5" ht="40.200000000000003" customHeight="1">
       <c r="A31" s="8"/>
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
     </row>
     <row r="32" spans="1:5" ht="25.95" customHeight="1">
       <c r="A32" s="7"/>
@@ -12352,12 +12352,12 @@
     </row>
     <row r="36" spans="1:5" ht="40.200000000000003" customHeight="1">
       <c r="A36" s="8"/>
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="48"/>
     </row>
     <row r="37" spans="1:5" ht="25.95" customHeight="1">
       <c r="B37" s="28" t="s">
@@ -12529,12 +12529,12 @@
     </row>
     <row r="48" spans="1:5" ht="40.200000000000003" customHeight="1">
       <c r="A48" s="8"/>
-      <c r="B48" s="47" t="s">
+      <c r="B48" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="47"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="47"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="48"/>
     </row>
     <row r="49" spans="1:5" ht="25.95" customHeight="1">
       <c r="A49" s="4"/>
@@ -12630,12 +12630,12 @@
     </row>
     <row r="55" spans="1:5" s="22" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A55" s="21"/>
-      <c r="B55" s="47" t="s">
+      <c r="B55" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="C55" s="47"/>
-      <c r="D55" s="47"/>
-      <c r="E55" s="47"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="48"/>
     </row>
     <row r="56" spans="1:5" ht="25.95" customHeight="1">
       <c r="B56" s="28" t="s">
@@ -12656,14 +12656,14 @@
         <v>105</v>
       </c>
       <c r="C57" s="34">
+        <v>25000</v>
+      </c>
+      <c r="D57" s="34">
         <v>20000</v>
-      </c>
-      <c r="D57" s="34">
-        <v>0</v>
       </c>
       <c r="E57" s="34">
         <f>Despesas!$C57-Despesas!$D57</f>
-        <v>20000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="25.95" customHeight="1">
@@ -12732,15 +12732,15 @@
       </c>
       <c r="C62" s="35">
         <f>SUBTOTAL(109,Decorações[ESTIMADO])</f>
-        <v>20000</v>
+        <v>25000</v>
       </c>
       <c r="D62" s="35">
         <f>SUBTOTAL(109,Decorações[REAL])</f>
-        <v>720</v>
+        <v>20720</v>
       </c>
       <c r="E62" s="35">
         <f>SUBTOTAL(109,Decorações[ACIMA/ABAIXO/RESTANTE])</f>
-        <v>19280</v>
+        <v>4280</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="25.95" customHeight="1">
@@ -12753,12 +12753,12 @@
     </row>
     <row r="64" spans="1:5" s="22" customFormat="1" ht="30" customHeight="1">
       <c r="A64" s="21"/>
-      <c r="B64" s="47" t="s">
+      <c r="B64" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
-      <c r="E64" s="47"/>
+      <c r="C64" s="48"/>
+      <c r="D64" s="48"/>
+      <c r="E64" s="48"/>
     </row>
     <row r="65" spans="1:5" ht="25.95" customHeight="1">
       <c r="B65" s="28" t="s">
@@ -12868,12 +12868,12 @@
     </row>
     <row r="72" spans="1:5" s="22" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A72" s="21"/>
-      <c r="B72" s="47" t="s">
+      <c r="B72" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="C72" s="47"/>
-      <c r="D72" s="47"/>
-      <c r="E72" s="47"/>
+      <c r="C72" s="48"/>
+      <c r="D72" s="48"/>
+      <c r="E72" s="48"/>
     </row>
     <row r="73" spans="1:5" ht="25.95" customHeight="1">
       <c r="B73" s="28" t="s">
@@ -12983,12 +12983,12 @@
     </row>
     <row r="80" spans="1:5" s="22" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A80" s="21"/>
-      <c r="B80" s="47" t="s">
+      <c r="B80" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="C80" s="47"/>
-      <c r="D80" s="47"/>
-      <c r="E80" s="47"/>
+      <c r="C80" s="48"/>
+      <c r="D80" s="48"/>
+      <c r="E80" s="48"/>
     </row>
     <row r="81" spans="1:5" ht="25.95" customHeight="1">
       <c r="B81" s="28" t="s">
@@ -13068,12 +13068,12 @@
     </row>
     <row r="86" spans="1:5" s="22" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A86" s="21"/>
-      <c r="B86" s="47" t="s">
+      <c r="B86" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="C86" s="47"/>
-      <c r="D86" s="47"/>
-      <c r="E86" s="47"/>
+      <c r="C86" s="48"/>
+      <c r="D86" s="48"/>
+      <c r="E86" s="48"/>
     </row>
     <row r="87" spans="1:5" ht="25.95" customHeight="1">
       <c r="B87" s="28" t="s">
@@ -13258,10 +13258,10 @@
     </row>
     <row r="99" spans="1:5" ht="16.2" customHeight="1">
       <c r="A99" s="8"/>
-      <c r="B99" s="44"/>
-      <c r="C99" s="44"/>
-      <c r="D99" s="44"/>
-      <c r="E99" s="44"/>
+      <c r="B99" s="45"/>
+      <c r="C99" s="45"/>
+      <c r="D99" s="45"/>
+      <c r="E99" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -13340,23 +13340,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13660,22 +13649,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E74ABAA7-A768-4083-B334-861CAEDB0669}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC9578A2-3FA9-45E5-AD32-3E5DFD27DB8E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13702,9 +13698,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC9578A2-3FA9-45E5-AD32-3E5DFD27DB8E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E74ABAA7-A768-4083-B334-861CAEDB0669}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>